<commit_message>
Add stations and catchments for CL Vestland project
</commit_message>
<xml_diff>
--- a/cl_vestland/cl_vestland_stns.xlsx
+++ b/cl_vestland/cl_vestland_stns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\316_MI_General\JupyterHub\niva_jupyter_hub\postgis_db\stn_proj_catch_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42891D61-7B28-4E3A-B56F-F5C52C9D9CE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECE7EDE-9384-459A-B3BC-FA718EC3C109}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{77F2D426-C92A-40CB-B2DA-14C4965D3DBB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>project_code</t>
   </si>
@@ -101,16 +101,25 @@
     <t>Samnanger_Frolandskanalen</t>
   </si>
   <si>
-    <t>/home/jovyan/projects/critical_loads_2/shapefiles/Samnanger_Tysseelva.shp</t>
-  </si>
-  <si>
-    <t>/home/jovyan/projects/critical_loads_2/shapefiles/Samnanger_Storelva.shp</t>
-  </si>
-  <si>
-    <t>/home/jovyan/projects/critical_loads_2/shapefiles/Samnanger_Frolandselva.shp</t>
-  </si>
-  <si>
-    <t>/home/jovyan/projects/critical_loads_2/shapefiles/Samnanger_Frolandskanalen_ny.shp</t>
+    <t>/home/jovyan/projects/critical_loads_2/cl_vestland/shapefiles/Samnanger.shp</t>
+  </si>
+  <si>
+    <t>/home/jovyan/projects/critical_loads_2/cl_vestland/shapefiles/Samnanger_Storelva.shp</t>
+  </si>
+  <si>
+    <t>/home/jovyan/projects/critical_loads_2/cl_vestland/shapefiles/Samnanger_Frolandselva.shp</t>
+  </si>
+  <si>
+    <t>/home/jovyan/projects/critical_loads_2/cl_vestland/shapefiles/Samnanger_Frolandskanalen_ny.shp</t>
+  </si>
+  <si>
+    <t>Samnanger_Tysseelva_Intercatchment</t>
+  </si>
+  <si>
+    <t>/home/jovyan/projects/critical_loads_2/cl_vestland/shapefiles/Samnanger_Tysseelva_ny.shp</t>
+  </si>
+  <si>
+    <t>Sam_Tyss_IntCat</t>
   </si>
 </sst>
 </file>
@@ -526,10 +535,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA92022-61C7-4FE3-977A-540D6B1F5F87}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -538,7 +547,7 @@
     <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.06640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="80.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -580,52 +589,69 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D3">
-        <v>5.7984426999999998</v>
+        <v>5.7585797999999997</v>
       </c>
       <c r="E3">
-        <v>60.384011299999997</v>
+        <v>60.3748991</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4">
-        <v>5.7985097999999997</v>
+        <v>5.7984426999999998</v>
       </c>
       <c r="E4">
-        <v>60.380058400000003</v>
+        <v>60.384011299999997</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>5.7985097999999997</v>
+      </c>
+      <c r="E5">
+        <v>60.380058400000003</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>5.7939176999999997</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>60.381434200000001</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Re-run with updated catchments
</commit_message>
<xml_diff>
--- a/cl_vestland/cl_vestland_stns.xlsx
+++ b/cl_vestland/cl_vestland_stns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\316_MI_General\JupyterHub\niva_jupyter_hub\postgis_db\stn_proj_catch_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECE7EDE-9384-459A-B3BC-FA718EC3C109}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3946BC-90F5-4284-B46D-25E4BDE114FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{77F2D426-C92A-40CB-B2DA-14C4965D3DBB}"/>
   </bookViews>
@@ -104,15 +104,9 @@
     <t>/home/jovyan/projects/critical_loads_2/cl_vestland/shapefiles/Samnanger.shp</t>
   </si>
   <si>
-    <t>/home/jovyan/projects/critical_loads_2/cl_vestland/shapefiles/Samnanger_Storelva.shp</t>
-  </si>
-  <si>
     <t>/home/jovyan/projects/critical_loads_2/cl_vestland/shapefiles/Samnanger_Frolandselva.shp</t>
   </si>
   <si>
-    <t>/home/jovyan/projects/critical_loads_2/cl_vestland/shapefiles/Samnanger_Frolandskanalen_ny.shp</t>
-  </si>
-  <si>
     <t>Samnanger_Tysseelva_Intercatchment</t>
   </si>
   <si>
@@ -120,6 +114,12 @@
   </si>
   <si>
     <t>Sam_Tyss_IntCat</t>
+  </si>
+  <si>
+    <t>/home/jovyan/projects/critical_loads_2/cl_vestland/shapefiles/Samnanger_Storelva_ny.shp</t>
+  </si>
+  <si>
+    <t>/home/jovyan/projects/critical_loads_2/cl_vestland/shapefiles/Samnanger_Frolandskanalen_nyere.shp</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -589,10 +589,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>5.7585797999999997</v>
@@ -601,7 +601,7 @@
         <v>60.3748991</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -618,7 +618,7 @@
         <v>60.384011299999997</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -635,7 +635,7 @@
         <v>60.380058400000003</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -652,7 +652,7 @@
         <v>60.381434200000001</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>